<commit_message>
create method to create new account
</commit_message>
<xml_diff>
--- a/Database Table/master_akun.xlsx
+++ b/Database Table/master_akun.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bidin\Documents\BELAJAR\C#\.NET\API\E-Learning.API\Database Table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramad\OneDrive\Documents\Belajar\.NET Web API\E-Learning-API\Database Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{090AD610-048E-4EB4-A44C-F012CA2AD520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AB42D2-5298-4A30-84CD-5F4253EAFC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{21B7923C-01C7-4CBD-8888-C131085446FF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{21B7923C-01C7-4CBD-8888-C131085446FF}"/>
   </bookViews>
   <sheets>
     <sheet name="master_akun" sheetId="2" r:id="rId1"/>
@@ -115,15 +115,21 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -162,11 +168,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E000D4D2-B2A9-4FF6-9FC5-C6EBA66CB509}" name="master_akun" displayName="master_akun" ref="A1:E4" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:E4" xr:uid="{E000D4D2-B2A9-4FF6-9FC5-C6EBA66CB509}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7F789308-D25D-4203-8FBA-9AA73007CDD8}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{D21C99B3-654D-4E55-A784-856B32F19356}" uniqueName="2" name="username" queryTableFieldId="2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{71480567-C709-4B17-8A9C-540750418811}" uniqueName="3" name="password" queryTableFieldId="3" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{120F4FA7-78E9-4FC1-8B62-76623E5D51BD}" uniqueName="4" name="tanggal_daftar" queryTableFieldId="4" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{B5B893B4-EFF8-4F5D-8974-96DA62579940}" uniqueName="5" name="id_peran" queryTableFieldId="5"/>
+    <tableColumn id="1" xr3:uid="{7F789308-D25D-4203-8FBA-9AA73007CDD8}" uniqueName="1" name="id" queryTableFieldId="1" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{D21C99B3-654D-4E55-A784-856B32F19356}" uniqueName="2" name="username" queryTableFieldId="2" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{71480567-C709-4B17-8A9C-540750418811}" uniqueName="3" name="password" queryTableFieldId="3" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{120F4FA7-78E9-4FC1-8B62-76623E5D51BD}" uniqueName="4" name="tanggal_daftar" queryTableFieldId="4" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{B5B893B4-EFF8-4F5D-8974-96DA62579940}" uniqueName="5" name="id_peran" queryTableFieldId="5" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -471,18 +477,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7147172-B787-423B-9495-98ED6B3E5FA9}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -499,54 +507,54 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>45125.453689155096</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>45125.453689155096</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>45125.453689155096</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>2</v>
       </c>
     </row>

</xml_diff>